<commit_message>
random forest scores, along with MLR score revisited
</commit_message>
<xml_diff>
--- a/revised_all_in_one.xlsx
+++ b/revised_all_in_one.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liu2286\Documents\GitHub\mdm_3_phace_C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FD1842-E986-4747-8C4F-788E8E52CBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB663B3-3B4C-4D5F-BB6B-68249DB55C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47037,8 +47037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP347"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AN11" sqref="AN11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -47048,6 +47048,10 @@
     <col min="9" max="9" width="21.625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.15">

</xml_diff>